<commit_message>
- Added: 1067-Fix-GLComponent-GLAccount: to fix GLAccount active status - Added: 1068-Fix-MR-GLAccount: to park MR/MRLine/InvUseLine/InvReserve under cost centre '0000000' if cost centre value from coswin is not active (start with '2x'). Coswin value is stored in custom column. Note: There is already a logic to do cost centre replacement. But the mapping is not yet provided by SBST. - Added: 1069-Fix-PO-GLAccount: to park PRLine/RFQLine/POLine/InvoiceCost under cost centre '0000000' if cost centre value from coswin is not active (start with '2x'). Coswin value is stored in custom column. Note: There is already a logic to do cost centre replacement. But the mapping is not yet provided by SBST. - Added: 1070-Fix-MR-Relationship: to set MR.MRSTATUSSEQ and MATUSETRANS.INVUSELINESPLITID
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/DM-COMPLETENESS-INTEGRITY.xlsx
+++ b/Integration Services Project2/notes/DM-COMPLETENESS-INTEGRITY.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044AC00C-187A-4F49-A4F9-539AAFBFB3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAB25FA-431A-404C-BB4D-E84A290784D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F4B014AE-0D6C-4ECE-9A76-61FA2F7E0A8C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F4B014AE-0D6C-4ECE-9A76-61FA2F7E0A8C}"/>
   </bookViews>
   <sheets>
     <sheet name="COSWIN" sheetId="1" r:id="rId1"/>
@@ -8009,6 +8009,11 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4604D927-7B6E-4B1D-9080-5EEA022272BF}" name="Table1" displayName="Table1" ref="A1:L538" totalsRowShown="0" dataDxfId="16">
   <autoFilter ref="A1:L538" xr:uid="{4604D927-7B6E-4B1D-9080-5EEA022272BF}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="RES_EMPL"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="6">
       <filters>
         <filter val="Ref"/>
@@ -8365,13 +8370,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A48D807-BC1E-4246-AEE5-B97976016A1C}">
-  <dimension ref="A1:L538"/>
+  <dimension ref="A1:L553"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <pane xSplit="6" ySplit="1" topLeftCell="G282" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K291" sqref="K291"/>
+      <selection pane="bottomRight" activeCell="K553" sqref="K553"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10669,7 +10674,7 @@
       </c>
       <c r="L72" s="8"/>
     </row>
-    <row r="73" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="8">
         <v>609</v>
       </c>
@@ -10732,7 +10737,7 @@
       <c r="J74" s="1"/>
       <c r="K74"/>
     </row>
-    <row r="75" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>611</v>
       </c>
@@ -11007,7 +11012,7 @@
       </c>
       <c r="L82" s="8"/>
     </row>
-    <row r="83" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="8">
         <v>619</v>
       </c>
@@ -11157,7 +11162,7 @@
       <c r="J87" s="1"/>
       <c r="K87"/>
     </row>
-    <row r="88" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="8">
         <v>624</v>
       </c>
@@ -11193,7 +11198,7 @@
       </c>
       <c r="L88" s="8"/>
     </row>
-    <row r="89" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="8">
         <v>625</v>
       </c>
@@ -11287,7 +11292,7 @@
       <c r="J91" s="1"/>
       <c r="K91"/>
     </row>
-    <row r="92" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="8">
         <v>628</v>
       </c>
@@ -11320,7 +11325,7 @@
       </c>
       <c r="L92" s="8"/>
     </row>
-    <row r="93" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="8">
         <v>629</v>
       </c>
@@ -11439,7 +11444,7 @@
       <c r="J96" s="1"/>
       <c r="K96"/>
     </row>
-    <row r="97" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="8">
         <v>633</v>
       </c>
@@ -11472,7 +11477,7 @@
       </c>
       <c r="L97" s="8"/>
     </row>
-    <row r="98" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="8">
         <v>634</v>
       </c>
@@ -11541,7 +11546,7 @@
       </c>
       <c r="L99" s="8"/>
     </row>
-    <row r="100" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="8">
         <v>636</v>
       </c>
@@ -11751,7 +11756,7 @@
       </c>
       <c r="L106" s="8"/>
     </row>
-    <row r="107" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>643</v>
       </c>
@@ -11782,7 +11787,7 @@
       </c>
       <c r="K107"/>
     </row>
-    <row r="108" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>644</v>
       </c>
@@ -11813,7 +11818,7 @@
       </c>
       <c r="K108"/>
     </row>
-    <row r="109" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="8">
         <v>645</v>
       </c>
@@ -11849,7 +11854,7 @@
       </c>
       <c r="L109" s="8"/>
     </row>
-    <row r="110" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="8">
         <v>646</v>
       </c>
@@ -11882,7 +11887,7 @@
       </c>
       <c r="L110" s="8"/>
     </row>
-    <row r="111" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="8">
         <v>647</v>
       </c>
@@ -12006,7 +12011,7 @@
       </c>
       <c r="L114" s="8"/>
     </row>
-    <row r="115" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="8">
         <v>651</v>
       </c>
@@ -12042,7 +12047,7 @@
       </c>
       <c r="L115" s="8"/>
     </row>
-    <row r="116" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="8">
         <v>652</v>
       </c>
@@ -12075,7 +12080,7 @@
       </c>
       <c r="L116" s="8"/>
     </row>
-    <row r="117" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="8">
         <v>653</v>
       </c>
@@ -12138,7 +12143,7 @@
       <c r="J118" s="1"/>
       <c r="K118"/>
     </row>
-    <row r="119" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>655</v>
       </c>
@@ -12263,7 +12268,7 @@
       </c>
       <c r="L122" s="8"/>
     </row>
-    <row r="123" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="8">
         <v>659</v>
       </c>
@@ -12368,7 +12373,7 @@
       </c>
       <c r="L125" s="8"/>
     </row>
-    <row r="126" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="8">
         <v>662</v>
       </c>
@@ -12516,7 +12521,7 @@
       </c>
       <c r="L130" s="8"/>
     </row>
-    <row r="131" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="8">
         <v>667</v>
       </c>
@@ -12724,7 +12729,7 @@
       <c r="J137" s="1"/>
       <c r="K137"/>
     </row>
-    <row r="138" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="8">
         <v>674</v>
       </c>
@@ -12814,7 +12819,7 @@
       <c r="J140" s="1"/>
       <c r="K140"/>
     </row>
-    <row r="141" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="8">
         <v>677</v>
       </c>
@@ -12847,7 +12852,7 @@
       </c>
       <c r="L141" s="8"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>678</v>
       </c>
@@ -12876,7 +12881,7 @@
       <c r="J142" s="1"/>
       <c r="K142"/>
     </row>
-    <row r="143" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="8">
         <v>679</v>
       </c>
@@ -12936,7 +12941,7 @@
       </c>
       <c r="K144"/>
     </row>
-    <row r="145" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="8">
         <v>681</v>
       </c>
@@ -12972,7 +12977,7 @@
       </c>
       <c r="L145" s="8"/>
     </row>
-    <row r="146" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="8">
         <v>682</v>
       </c>
@@ -13005,7 +13010,7 @@
       </c>
       <c r="L146" s="8"/>
     </row>
-    <row r="147" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="8">
         <v>683</v>
       </c>
@@ -13065,7 +13070,7 @@
       <c r="J148" s="1"/>
       <c r="K148"/>
     </row>
-    <row r="149" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>685</v>
       </c>
@@ -13094,7 +13099,7 @@
       <c r="J149" s="1"/>
       <c r="K149"/>
     </row>
-    <row r="150" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>686</v>
       </c>
@@ -13152,7 +13157,7 @@
       <c r="J151" s="1"/>
       <c r="K151"/>
     </row>
-    <row r="152" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="8">
         <v>688</v>
       </c>
@@ -13188,7 +13193,7 @@
       </c>
       <c r="L152" s="8"/>
     </row>
-    <row r="153" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="8">
         <v>689</v>
       </c>
@@ -13275,7 +13280,7 @@
       <c r="J155" s="1"/>
       <c r="K155"/>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>692</v>
       </c>
@@ -13304,7 +13309,7 @@
       <c r="J156" s="1"/>
       <c r="K156" s="1"/>
     </row>
-    <row r="157" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="8">
         <v>693</v>
       </c>
@@ -13467,7 +13472,7 @@
       <c r="J162" s="1"/>
       <c r="K162"/>
     </row>
-    <row r="163" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="8">
         <v>699</v>
       </c>
@@ -13828,7 +13833,7 @@
       <c r="J175" s="1"/>
       <c r="K175"/>
     </row>
-    <row r="176" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" s="8">
         <v>712</v>
       </c>
@@ -13972,7 +13977,7 @@
       </c>
       <c r="L180" s="8"/>
     </row>
-    <row r="181" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" s="8">
         <v>717</v>
       </c>
@@ -15697,7 +15702,7 @@
       <c r="J240" s="1"/>
       <c r="K240"/>
     </row>
-    <row r="241" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" s="8">
         <v>777</v>
       </c>
@@ -15891,7 +15896,7 @@
       </c>
       <c r="L247" s="8"/>
     </row>
-    <row r="248" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" s="8">
         <v>784</v>
       </c>
@@ -16082,7 +16087,7 @@
       </c>
       <c r="L253" s="8"/>
     </row>
-    <row r="254" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" s="8">
         <v>790</v>
       </c>
@@ -16113,7 +16118,7 @@
       </c>
       <c r="L254" s="8"/>
     </row>
-    <row r="255" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" s="8">
         <v>791</v>
       </c>
@@ -16146,7 +16151,7 @@
       </c>
       <c r="L255" s="8"/>
     </row>
-    <row r="256" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" s="8">
         <v>792</v>
       </c>
@@ -16179,7 +16184,7 @@
       </c>
       <c r="L256" s="8"/>
     </row>
-    <row r="257" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" s="8">
         <v>793</v>
       </c>
@@ -16212,7 +16217,7 @@
       </c>
       <c r="L257" s="8"/>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>794</v>
       </c>
@@ -16277,7 +16282,7 @@
       </c>
       <c r="L259" s="8"/>
     </row>
-    <row r="260" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" s="8">
         <v>796</v>
       </c>
@@ -16380,7 +16385,7 @@
       </c>
       <c r="L262" s="8"/>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" s="8">
         <v>799</v>
       </c>
@@ -16458,7 +16463,7 @@
       <c r="J265" s="1"/>
       <c r="K265"/>
     </row>
-    <row r="266" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" s="8">
         <v>802</v>
       </c>
@@ -16494,7 +16499,7 @@
       </c>
       <c r="L266" s="8"/>
     </row>
-    <row r="267" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" s="8">
         <v>803</v>
       </c>
@@ -16558,7 +16563,7 @@
       </c>
       <c r="L268" s="8"/>
     </row>
-    <row r="269" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269" s="8">
         <v>805</v>
       </c>
@@ -16674,7 +16679,7 @@
       <c r="J272" s="1"/>
       <c r="K272"/>
     </row>
-    <row r="273" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:12" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273" s="8">
         <v>809</v>
       </c>
@@ -16832,7 +16837,7 @@
       <c r="J278" s="1"/>
       <c r="K278"/>
     </row>
-    <row r="279" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:12" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" s="8">
         <v>815</v>
       </c>
@@ -16890,7 +16895,7 @@
       <c r="J280" s="1"/>
       <c r="K280"/>
     </row>
-    <row r="281" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281" s="8">
         <v>817</v>
       </c>
@@ -16923,7 +16928,7 @@
       </c>
       <c r="L281" s="8"/>
     </row>
-    <row r="282" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" s="8">
         <v>818</v>
       </c>
@@ -17173,7 +17178,7 @@
       <c r="J290" s="1"/>
       <c r="K290"/>
     </row>
-    <row r="291" spans="1:12" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:12" ht="244.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" s="8">
         <v>827</v>
       </c>
@@ -18034,7 +18039,7 @@
       <c r="J323" s="1"/>
       <c r="K323"/>
     </row>
-    <row r="324" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324" s="8">
         <v>860</v>
       </c>
@@ -18183,7 +18188,7 @@
       <c r="J328" s="1"/>
       <c r="K328"/>
     </row>
-    <row r="329" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A329" s="8">
         <v>865</v>
       </c>
@@ -19025,7 +19030,7 @@
       <c r="J360" s="1"/>
       <c r="K360"/>
     </row>
-    <row r="361" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A361">
         <v>897</v>
       </c>
@@ -19266,7 +19271,7 @@
       <c r="J369" s="1"/>
       <c r="K369"/>
     </row>
-    <row r="370" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A370" s="8">
         <v>906</v>
       </c>
@@ -19338,7 +19343,7 @@
       </c>
       <c r="L371" s="8"/>
     </row>
-    <row r="372" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A372" s="8">
         <v>908</v>
       </c>
@@ -19443,7 +19448,7 @@
       </c>
       <c r="L374" s="8"/>
     </row>
-    <row r="375" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A375" s="8">
         <v>911</v>
       </c>
@@ -19474,7 +19479,7 @@
       </c>
       <c r="L375" s="8"/>
     </row>
-    <row r="376" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A376" s="8">
         <v>912</v>
       </c>
@@ -19543,7 +19548,7 @@
       </c>
       <c r="L377" s="8"/>
     </row>
-    <row r="378" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A378">
         <v>914</v>
       </c>
@@ -19599,7 +19604,7 @@
       <c r="J379" s="1"/>
       <c r="K379"/>
     </row>
-    <row r="380" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A380" s="8">
         <v>916</v>
       </c>
@@ -19704,7 +19709,7 @@
       </c>
       <c r="L382" s="8"/>
     </row>
-    <row r="383" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A383" s="8">
         <v>919</v>
       </c>
@@ -19771,7 +19776,7 @@
       </c>
       <c r="L384" s="8"/>
     </row>
-    <row r="385" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:12" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A385" s="8">
         <v>921</v>
       </c>
@@ -19868,7 +19873,7 @@
       </c>
       <c r="L387" s="8"/>
     </row>
-    <row r="388" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A388" s="8">
         <v>924</v>
       </c>
@@ -19959,7 +19964,7 @@
       <c r="J390" s="1"/>
       <c r="K390"/>
     </row>
-    <row r="391" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A391">
         <v>927</v>
       </c>
@@ -20348,7 +20353,7 @@
       <c r="J404" s="1"/>
       <c r="K404"/>
     </row>
-    <row r="405" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A405" s="8">
         <v>941</v>
       </c>
@@ -20499,7 +20504,7 @@
       <c r="J409" s="1"/>
       <c r="K409"/>
     </row>
-    <row r="410" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A410" s="8">
         <v>946</v>
       </c>
@@ -20532,7 +20537,7 @@
       </c>
       <c r="L410" s="8"/>
     </row>
-    <row r="411" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A411" s="8">
         <v>947</v>
       </c>
@@ -20615,7 +20620,7 @@
       <c r="J413" s="1"/>
       <c r="K413"/>
     </row>
-    <row r="414" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A414">
         <v>950</v>
       </c>
@@ -20707,7 +20712,7 @@
       <c r="J416" s="1"/>
       <c r="K416"/>
     </row>
-    <row r="417" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A417">
         <v>953</v>
       </c>
@@ -20963,7 +20968,7 @@
       <c r="J426" s="1"/>
       <c r="K426"/>
     </row>
-    <row r="427" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A427" s="8">
         <v>963</v>
       </c>
@@ -20996,7 +21001,7 @@
       </c>
       <c r="L427" s="8"/>
     </row>
-    <row r="428" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A428">
         <v>964</v>
       </c>
@@ -21052,7 +21057,7 @@
       <c r="J429" s="1"/>
       <c r="K429"/>
     </row>
-    <row r="430" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A430" s="8">
         <v>966</v>
       </c>
@@ -21146,7 +21151,7 @@
       </c>
       <c r="L432" s="8"/>
     </row>
-    <row r="433" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A433" s="8">
         <v>969</v>
       </c>
@@ -21179,7 +21184,7 @@
       </c>
       <c r="L433" s="8"/>
     </row>
-    <row r="434" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A434" s="8">
         <v>970</v>
       </c>
@@ -21245,7 +21250,7 @@
       </c>
       <c r="L435" s="8"/>
     </row>
-    <row r="436" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A436">
         <v>972</v>
       </c>
@@ -21274,7 +21279,7 @@
       <c r="J436" s="1"/>
       <c r="K436"/>
     </row>
-    <row r="437" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A437" s="8">
         <v>973</v>
       </c>
@@ -21305,7 +21310,7 @@
       </c>
       <c r="L437" s="8"/>
     </row>
-    <row r="438" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A438" s="8">
         <v>974</v>
       </c>
@@ -21338,7 +21343,7 @@
       </c>
       <c r="L438" s="8"/>
     </row>
-    <row r="439" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A439" s="8">
         <v>975</v>
       </c>
@@ -21371,7 +21376,7 @@
       </c>
       <c r="L439" s="8"/>
     </row>
-    <row r="440" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A440" s="8">
         <v>976</v>
       </c>
@@ -21401,7 +21406,7 @@
       </c>
       <c r="L440" s="8"/>
     </row>
-    <row r="441" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A441" s="8">
         <v>977</v>
       </c>
@@ -21817,7 +21822,7 @@
       </c>
       <c r="L453" s="8"/>
     </row>
-    <row r="454" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A454">
         <v>990</v>
       </c>
@@ -21871,7 +21876,7 @@
       <c r="J455" s="1"/>
       <c r="K455"/>
     </row>
-    <row r="456" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:12" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A456" s="8">
         <v>992</v>
       </c>
@@ -23407,7 +23412,7 @@
       <c r="J511" s="1"/>
       <c r="K511"/>
     </row>
-    <row r="512" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="512" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A512" s="8">
         <v>1048</v>
       </c>
@@ -23440,7 +23445,7 @@
       </c>
       <c r="L512" s="8"/>
     </row>
-    <row r="513" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A513" s="8">
         <v>1049</v>
       </c>
@@ -23655,7 +23660,7 @@
       <c r="J520" s="1"/>
       <c r="K520"/>
     </row>
-    <row r="521" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="521" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A521" s="8">
         <v>1057</v>
       </c>
@@ -23688,7 +23693,7 @@
       </c>
       <c r="L521" s="8"/>
     </row>
-    <row r="522" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="522" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A522">
         <v>1058</v>
       </c>
@@ -23719,7 +23724,7 @@
       </c>
       <c r="K522"/>
     </row>
-    <row r="523" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="523" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A523">
         <v>1059</v>
       </c>
@@ -23750,7 +23755,7 @@
       </c>
       <c r="K523"/>
     </row>
-    <row r="524" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="524" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A524" s="8">
         <v>1060</v>
       </c>
@@ -23783,7 +23788,7 @@
       </c>
       <c r="L524" s="8"/>
     </row>
-    <row r="525" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="525" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A525" s="8">
         <v>1061</v>
       </c>
@@ -23814,7 +23819,7 @@
       </c>
       <c r="L525" s="8"/>
     </row>
-    <row r="526" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="526" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A526" s="8">
         <v>1062</v>
       </c>
@@ -23933,7 +23938,7 @@
       </c>
       <c r="L529" s="8"/>
     </row>
-    <row r="530" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="530" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A530" s="8">
         <v>1066</v>
       </c>
@@ -24204,6 +24209,34 @@
         <v>2354</v>
       </c>
       <c r="L538" s="8"/>
+    </row>
+    <row r="550" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J550" s="9">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="551" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J551" s="9">
+        <v>783</v>
+      </c>
+      <c r="K551" s="9">
+        <f>J551+J550</f>
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="552" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J552" s="9">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="553" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J553" s="9">
+        <v>1117</v>
+      </c>
+      <c r="K553" s="9">
+        <f>J553+J552</f>
+        <v>1815</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24217,7 +24250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3561533-4E1B-4993-86F5-1EB6A8739D3E}">
   <dimension ref="A1:E182"/>
   <sheetViews>
-    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>